<commit_message>
int->uint32_t und progress.sh hinzugefügt
</commit_message>
<xml_diff>
--- a/ex_03/ex_01/scripts/Jacobi.xlsx
+++ b/ex_03/ex_01/scripts/Jacobi.xlsx
@@ -863,6 +863,7 @@
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -2364,13 +2365,13 @@
         <v>512</v>
       </c>
       <c r="C2">
-        <v>31.325710999999998</v>
+        <v>31.266141999999999</v>
       </c>
       <c r="D2">
-        <v>29.301317999999998</v>
+        <v>29.156341000000001</v>
       </c>
       <c r="E2">
-        <v>30.879816999999999</v>
+        <v>30.723811000000001</v>
       </c>
       <c r="G2"/>
       <c r="I2"/>
@@ -2385,13 +2386,13 @@
         <v>648</v>
       </c>
       <c r="C3">
-        <v>41.621181999999997</v>
+        <v>41.505144000000001</v>
       </c>
       <c r="D3">
-        <v>37.888378000000003</v>
+        <v>37.727808000000003</v>
       </c>
       <c r="E3">
-        <v>40.990727999999997</v>
+        <v>40.65052</v>
       </c>
       <c r="G3"/>
       <c r="I3"/>
@@ -2406,13 +2407,13 @@
         <v>968</v>
       </c>
       <c r="C4">
-        <v>64.766913000000002</v>
+        <v>64.771221999999995</v>
       </c>
       <c r="D4">
-        <v>57.117578000000002</v>
+        <v>56.81127</v>
       </c>
       <c r="E4">
-        <v>63.711737999999997</v>
+        <v>63.433995000000003</v>
       </c>
       <c r="G4"/>
       <c r="I4"/>
@@ -2427,13 +2428,13 @@
         <v>1568</v>
       </c>
       <c r="C5">
-        <v>104.538512</v>
+        <v>104.279394</v>
       </c>
       <c r="D5">
-        <v>88.126926999999995</v>
+        <v>87.731187000000006</v>
       </c>
       <c r="E5">
-        <v>102.726179</v>
+        <v>102.491349</v>
       </c>
       <c r="G5"/>
       <c r="I5"/>
@@ -2448,13 +2449,13 @@
         <v>2312</v>
       </c>
       <c r="C6">
-        <v>147.18471500000001</v>
+        <v>146.37685400000001</v>
       </c>
       <c r="D6">
-        <v>115.136905</v>
+        <v>114.772543</v>
       </c>
       <c r="E6">
-        <v>143.14184299999999</v>
+        <v>142.70301000000001</v>
       </c>
       <c r="G6"/>
       <c r="I6"/>
@@ -2469,13 +2470,13 @@
         <v>3200</v>
       </c>
       <c r="C7">
-        <v>189.21018599999999</v>
+        <v>188.47886600000001</v>
       </c>
       <c r="D7">
-        <v>141.443364</v>
+        <v>141.28376299999999</v>
       </c>
       <c r="E7">
-        <v>185.27226400000001</v>
+        <v>184.880695</v>
       </c>
       <c r="G7"/>
       <c r="I7"/>
@@ -2490,13 +2491,13 @@
         <v>5000</v>
       </c>
       <c r="C8">
-        <v>252.647288</v>
+        <v>252.04335599999999</v>
       </c>
       <c r="D8">
-        <v>171.53703899999999</v>
+        <v>171.39779200000001</v>
       </c>
       <c r="E8">
-        <v>242.837152</v>
+        <v>242.61525399999999</v>
       </c>
       <c r="G8"/>
       <c r="I8"/>
@@ -2511,13 +2512,13 @@
         <v>7200</v>
       </c>
       <c r="C9">
-        <v>304.70307400000002</v>
+        <v>304.52142300000003</v>
       </c>
       <c r="D9">
-        <v>198.23767900000001</v>
+        <v>197.98104000000001</v>
       </c>
       <c r="E9">
-        <v>293.90658400000001</v>
+        <v>293.686892</v>
       </c>
       <c r="G9"/>
       <c r="I9"/>
@@ -2532,13 +2533,13 @@
         <v>10368</v>
       </c>
       <c r="C10">
-        <v>351.69925499999999</v>
+        <v>351.88000499999998</v>
       </c>
       <c r="D10">
-        <v>218.534468</v>
+        <v>218.28777299999999</v>
       </c>
       <c r="E10">
-        <v>344.356694</v>
+        <v>343.788093</v>
       </c>
       <c r="G10"/>
       <c r="I10"/>
@@ -2553,13 +2554,13 @@
         <v>15488</v>
       </c>
       <c r="C11">
-        <v>373.00507499999998</v>
+        <v>371.44203900000002</v>
       </c>
       <c r="D11">
-        <v>235.21671499999999</v>
+        <v>235.07004699999999</v>
       </c>
       <c r="E11">
-        <v>388.37993399999999</v>
+        <v>387.80200500000001</v>
       </c>
       <c r="G11"/>
       <c r="I11"/>
@@ -2574,13 +2575,13 @@
         <v>22472</v>
       </c>
       <c r="C12">
-        <v>409.487281</v>
+        <v>408.55467499999997</v>
       </c>
       <c r="D12">
-        <v>244.00628900000001</v>
+        <v>243.923001</v>
       </c>
       <c r="E12">
-        <v>409.81940400000002</v>
+        <v>409.43760099999997</v>
       </c>
       <c r="G12"/>
       <c r="I12"/>
@@ -2595,13 +2596,13 @@
         <v>32768</v>
       </c>
       <c r="C13">
-        <v>435.10860100000002</v>
+        <v>434.46960799999999</v>
       </c>
       <c r="D13">
-        <v>258.04052899999999</v>
+        <v>257.77111400000001</v>
       </c>
       <c r="E13">
-        <v>448.05178999999998</v>
+        <v>447.594134</v>
       </c>
       <c r="G13"/>
       <c r="I13"/>
@@ -2616,13 +2617,13 @@
         <v>48672</v>
       </c>
       <c r="C14">
-        <v>464.13924800000001</v>
+        <v>464.056668</v>
       </c>
       <c r="D14">
-        <v>264.563064</v>
+        <v>264.25369000000001</v>
       </c>
       <c r="E14">
-        <v>472.56390699999997</v>
+        <v>472.26501200000001</v>
       </c>
       <c r="G14"/>
       <c r="I14"/>
@@ -2637,13 +2638,13 @@
         <v>70688</v>
       </c>
       <c r="C15">
-        <v>482.631508</v>
+        <v>482.42541799999998</v>
       </c>
       <c r="D15">
-        <v>269.192432</v>
+        <v>269.038995</v>
       </c>
       <c r="E15">
-        <v>488.28701000000001</v>
+        <v>487.276499</v>
       </c>
       <c r="G15"/>
       <c r="I15"/>
@@ -2658,13 +2659,13 @@
         <v>103968</v>
       </c>
       <c r="C16">
-        <v>496.24983300000002</v>
+        <v>495.74538999999999</v>
       </c>
       <c r="D16">
-        <v>272.60178400000001</v>
+        <v>272.66361499999999</v>
       </c>
       <c r="E16">
-        <v>498.772626</v>
+        <v>497.858316</v>
       </c>
       <c r="G16"/>
       <c r="I16"/>
@@ -2679,13 +2680,13 @@
         <v>152352</v>
       </c>
       <c r="C17">
-        <v>434.79495800000001</v>
+        <v>430.24722600000001</v>
       </c>
       <c r="D17">
-        <v>271.29861599999998</v>
+        <v>272.41679699999997</v>
       </c>
       <c r="E17">
-        <v>495.51459399999999</v>
+        <v>497.24823800000001</v>
       </c>
       <c r="G17"/>
       <c r="I17"/>
@@ -2700,13 +2701,13 @@
         <v>223112</v>
       </c>
       <c r="C18">
-        <v>444.25807099999997</v>
+        <v>442.66938299999998</v>
       </c>
       <c r="D18">
-        <v>274.48812500000003</v>
+        <v>275.37886900000001</v>
       </c>
       <c r="E18">
-        <v>508.08388600000001</v>
+        <v>508.47377599999999</v>
       </c>
       <c r="G18"/>
       <c r="I18"/>
@@ -2721,13 +2722,13 @@
         <v>326432</v>
       </c>
       <c r="C19">
-        <v>441.90680200000003</v>
+        <v>444.35719799999998</v>
       </c>
       <c r="D19">
-        <v>276.21695399999999</v>
+        <v>276.54771299999999</v>
       </c>
       <c r="E19">
-        <v>513.46040400000004</v>
+        <v>512.74819400000001</v>
       </c>
       <c r="G19"/>
       <c r="I19"/>
@@ -2742,13 +2743,13 @@
         <v>476288</v>
       </c>
       <c r="C20">
-        <v>449.754324</v>
+        <v>450.687095</v>
       </c>
       <c r="D20">
-        <v>278.10727200000002</v>
+        <v>279.03792199999998</v>
       </c>
       <c r="E20">
-        <v>523.52781900000002</v>
+        <v>522.61687900000004</v>
       </c>
       <c r="G20"/>
       <c r="I20"/>
@@ -2763,13 +2764,13 @@
         <v>700928</v>
       </c>
       <c r="C21">
-        <v>452.91166399999997</v>
+        <v>446.87505900000002</v>
       </c>
       <c r="D21">
-        <v>280.00932699999998</v>
+        <v>279.752475</v>
       </c>
       <c r="E21">
-        <v>529.12314800000001</v>
+        <v>528.99499500000002</v>
       </c>
       <c r="G21"/>
       <c r="I21"/>
@@ -2784,13 +2785,13 @@
         <v>1025312</v>
       </c>
       <c r="C22">
-        <v>451.41153800000001</v>
+        <v>454.676401</v>
       </c>
       <c r="D22">
-        <v>279.959609</v>
+        <v>280.15740699999998</v>
       </c>
       <c r="E22">
-        <v>527.26195299999995</v>
+        <v>528.63598300000001</v>
       </c>
       <c r="G22"/>
       <c r="I22"/>
@@ -2805,13 +2806,13 @@
         <v>1492992</v>
       </c>
       <c r="C23">
-        <v>456.51772499999998</v>
+        <v>456.630244</v>
       </c>
       <c r="D23">
-        <v>280.94796400000001</v>
+        <v>281.22544299999998</v>
       </c>
       <c r="E23">
-        <v>532.94302300000004</v>
+        <v>533.30421999999999</v>
       </c>
       <c r="G23"/>
       <c r="I23"/>
@@ -2826,13 +2827,13 @@
         <v>2188232</v>
       </c>
       <c r="C24">
-        <v>457.346678</v>
+        <v>457.42714999999998</v>
       </c>
       <c r="D24">
-        <v>281.82542999999998</v>
+        <v>281.96346399999999</v>
       </c>
       <c r="E24">
-        <v>535.05069500000002</v>
+        <v>535.63520900000003</v>
       </c>
       <c r="G24"/>
       <c r="I24"/>
@@ -2847,13 +2848,13 @@
         <v>3205512</v>
       </c>
       <c r="C25">
-        <v>459.05774700000001</v>
+        <v>459.87224099999997</v>
       </c>
       <c r="D25">
-        <v>282.67763300000001</v>
+        <v>282.62504999999999</v>
       </c>
       <c r="E25">
-        <v>536.08799399999998</v>
+        <v>536.29155100000003</v>
       </c>
       <c r="G25"/>
       <c r="I25"/>
@@ -2868,13 +2869,13 @@
         <v>4681800</v>
       </c>
       <c r="C26">
-        <v>461.42947800000002</v>
+        <v>463.96293100000003</v>
       </c>
       <c r="D26">
-        <v>283.04281600000002</v>
+        <v>283.26708100000002</v>
       </c>
       <c r="E26">
-        <v>537.82707600000003</v>
+        <v>538.122254</v>
       </c>
       <c r="G26"/>
       <c r="I26"/>
@@ -2889,13 +2890,13 @@
         <v>6845000</v>
       </c>
       <c r="C27">
-        <v>464.75595299999998</v>
+        <v>464.68455599999999</v>
       </c>
       <c r="D27">
-        <v>283.547324</v>
+        <v>283.764634</v>
       </c>
       <c r="E27">
-        <v>539.59180400000002</v>
+        <v>540.00916299999994</v>
       </c>
       <c r="G27"/>
       <c r="I27"/>
@@ -2910,13 +2911,13 @@
         <v>10017288</v>
       </c>
       <c r="C28">
-        <v>462.58804500000002</v>
+        <v>462.33331600000002</v>
       </c>
       <c r="D28">
-        <v>283.63592799999998</v>
+        <v>283.92195900000002</v>
       </c>
       <c r="E28">
-        <v>540.05512899999997</v>
+        <v>540.653504</v>
       </c>
       <c r="G28"/>
       <c r="I28"/>
@@ -2931,13 +2932,13 @@
         <v>14666528</v>
       </c>
       <c r="C29">
-        <v>455.65303799999998</v>
+        <v>456.14648899999997</v>
       </c>
       <c r="D29">
-        <v>281.41463599999997</v>
+        <v>282.12787200000002</v>
       </c>
       <c r="E29">
-        <v>525.99317699999995</v>
+        <v>526.93032400000004</v>
       </c>
       <c r="G29"/>
       <c r="I29"/>
@@ -2952,13 +2953,13 @@
         <v>21438152</v>
       </c>
       <c r="C30">
-        <v>450.255177</v>
+        <v>451.443916</v>
       </c>
       <c r="D30">
-        <v>282.18510600000002</v>
+        <v>283.12654700000002</v>
       </c>
       <c r="E30">
-        <v>516.86345100000005</v>
+        <v>519.38055299999996</v>
       </c>
       <c r="G30"/>
       <c r="I30"/>
@@ -2973,13 +2974,13 @@
         <v>31363200</v>
       </c>
       <c r="C31">
-        <v>449.92936800000001</v>
+        <v>451.80636099999998</v>
       </c>
       <c r="D31">
-        <v>281.114915</v>
+        <v>281.82755600000002</v>
       </c>
       <c r="E31">
-        <v>505.14774799999998</v>
+        <v>508.023279</v>
       </c>
       <c r="G31"/>
       <c r="I31"/>
@@ -2994,13 +2995,13 @@
         <v>45849888</v>
       </c>
       <c r="C32">
-        <v>447.55753499999997</v>
+        <v>448.755492</v>
       </c>
       <c r="D32">
-        <v>280.239374</v>
+        <v>281.36632500000002</v>
       </c>
       <c r="E32">
-        <v>507.68298600000003</v>
+        <v>509.58154300000001</v>
       </c>
       <c r="G32"/>
       <c r="I32"/>
@@ -3015,13 +3016,13 @@
         <v>67094528</v>
       </c>
       <c r="C33">
-        <v>449.50554499999998</v>
+        <v>451.18319000000002</v>
       </c>
       <c r="D33">
-        <v>280.531204</v>
+        <v>281.68836199999998</v>
       </c>
       <c r="E33">
-        <v>505.93352399999998</v>
+        <v>505.17877399999998</v>
       </c>
       <c r="G33"/>
       <c r="I33"/>

</xml_diff>